<commit_message>
Added quiz data responses, home practice completion, engagement by week segregation
</commit_message>
<xml_diff>
--- a/PfR_Shiny.xlsx
+++ b/PfR_Shiny.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="134">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -415,6 +415,18 @@
   </si>
   <si>
     <t xml:space="preserve">session_completion_data_week </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Practice Completion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hp_done_data_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz Responses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quiz_done_data</t>
   </si>
 </sst>
 </file>
@@ -425,7 +437,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -512,12 +524,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -565,7 +571,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -620,10 +626,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1701,7 +1703,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1787,7 +1789,7 @@
       <c r="B8" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1802,8 +1804,28 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Updated PfR Dashboard 21.02.2025
</commit_message>
<xml_diff>
--- a/PfR_Shiny.xlsx
+++ b/PfR_Shiny.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="134">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -150,15 +150,6 @@
     <t xml:space="preserve">rp-contact-field._app_version</t>
   </si>
   <si>
-    <t xml:space="preserve">text = "App Language", colour = "blue"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">labs(x = "Language", y = "Count of Users")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rp-contact-field._app_language</t>
-  </si>
-  <si>
     <t xml:space="preserve">text = "Gender", colour = "blue"</t>
   </si>
   <si>
@@ -399,22 +390,31 @@
     <t xml:space="preserve">plhdata_org_download </t>
   </si>
   <si>
-    <t xml:space="preserve">Session Completion Longer</t>
+    <t xml:space="preserve">Session Completion Summary Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">session_completion_summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Session Completion per User Longer</t>
   </si>
   <si>
     <t xml:space="preserve">session_completion_longer</t>
   </si>
   <si>
+    <t xml:space="preserve">Session Completion per User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Session Completion Data Week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">session_completion_data_week </t>
+  </si>
+  <si>
     <t xml:space="preserve">Frequent Sessions per User</t>
   </si>
   <si>
     <t xml:space="preserve">frequent_sessions_per_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Session Completion Data Week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">session_completion_data_week </t>
   </si>
   <si>
     <t xml:space="preserve">Home Practice Completion</t>
@@ -955,10 +955,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
@@ -1056,24 +1056,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="F4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>46</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="n">
@@ -1085,40 +1085,42 @@
         <v>36</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
         <v>53</v>
       </c>
@@ -1132,54 +1134,29 @@
       <c r="A7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>37</v>
+      <c r="B7" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="F7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4" t="n">
         <v>4</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1198,8 +1175,8 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1257,13 +1234,13 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J2" s="4" t="n">
         <v>1</v>
@@ -1277,13 +1254,13 @@
         <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J3" s="4" t="n">
         <v>1</v>
@@ -1297,13 +1274,13 @@
         <v>37</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J4" s="4" t="n">
         <v>2</v>
@@ -1317,13 +1294,13 @@
         <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J5" s="4" t="n">
         <v>2</v>
@@ -1337,13 +1314,13 @@
         <v>37</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J6" s="4" t="n">
         <v>3</v>
@@ -1357,13 +1334,13 @@
         <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J7" s="4" t="n">
         <v>3</v>
@@ -1377,13 +1354,13 @@
         <v>37</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J8" s="4" t="n">
         <v>4</v>
@@ -1397,13 +1374,13 @@
         <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J9" s="4" t="n">
         <v>4</v>
@@ -1417,13 +1394,13 @@
         <v>37</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J10" s="4" t="n">
         <v>5</v>
@@ -1437,13 +1414,13 @@
         <v>37</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J11" s="4" t="n">
         <v>5</v>
@@ -1457,13 +1434,13 @@
         <v>37</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J12" s="4" t="n">
         <v>6</v>
@@ -1477,13 +1454,13 @@
         <v>37</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J13" s="4" t="n">
         <v>6</v>
@@ -1497,13 +1474,13 @@
         <v>37</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J14" s="4" t="n">
         <v>7</v>
@@ -1517,13 +1494,13 @@
         <v>37</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J15" s="4" t="n">
         <v>7</v>
@@ -1537,13 +1514,13 @@
         <v>37</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J16" s="4" t="n">
         <v>8</v>
@@ -1557,13 +1534,13 @@
         <v>37</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J17" s="4" t="n">
         <v>8</v>
@@ -1577,13 +1554,13 @@
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J18" s="4" t="n">
         <v>9</v>
@@ -1608,7 +1585,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1658,7 +1635,7 @@
         <v>35</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1666,22 +1643,22 @@
         <v>36</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1700,16 +1677,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.54"/>
   </cols>
@@ -1727,15 +1704,15 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>12</v>
@@ -1743,51 +1720,51 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>124</v>
-      </c>
       <c r="C6" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -1795,41 +1772,52 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C12" s="0" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added date filter variable/reworded hp done 03/03/2025
</commit_message>
<xml_diff>
--- a/PfR_Shiny.xlsx
+++ b/PfR_Shiny.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="138">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t xml:space="preserve">synced_more_than_30_days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_range_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label = "Choose your Date:", start = as.Date("2025-01-01") </t>
+  </si>
+  <si>
+    <t xml:space="preserve">createdAt </t>
   </si>
   <si>
     <t xml:space="preserve">table_manip</t>
@@ -571,7 +583,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -604,6 +616,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -622,10 +642,6 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -824,16 +840,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="69.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="68.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.54"/>
@@ -939,6 +956,23 @@
         <v>23</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -977,54 +1011,54 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="D1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>35</v>
+      <c r="H1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1034,21 +1068,21 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1058,20 +1092,20 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -1082,21 +1116,21 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -1106,23 +1140,23 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1132,22 +1166,22 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1175,7 +1209,7 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1194,53 +1228,53 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="4" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+    <row r="1" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="10" t="s">
+      <c r="D1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>35</v>
+      <c r="H1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="J2" s="4" t="n">
         <v>1</v>
@@ -1248,19 +1282,19 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="J3" s="4" t="n">
         <v>1</v>
@@ -1268,19 +1302,19 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="J4" s="4" t="n">
         <v>2</v>
@@ -1288,19 +1322,19 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="J5" s="4" t="n">
         <v>2</v>
@@ -1308,19 +1342,19 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="J6" s="4" t="n">
         <v>3</v>
@@ -1328,19 +1362,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>74</v>
+        <v>77</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="J7" s="4" t="n">
         <v>3</v>
@@ -1348,19 +1382,19 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="J8" s="4" t="n">
         <v>4</v>
@@ -1368,19 +1402,19 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>80</v>
+        <v>83</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="J9" s="4" t="n">
         <v>4</v>
@@ -1388,19 +1422,19 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>83</v>
+        <v>86</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="J10" s="4" t="n">
         <v>5</v>
@@ -1408,19 +1442,19 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>86</v>
+        <v>89</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="J11" s="4" t="n">
         <v>5</v>
@@ -1428,19 +1462,19 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>89</v>
+        <v>92</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="J12" s="4" t="n">
         <v>6</v>
@@ -1448,19 +1482,19 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>92</v>
+        <v>95</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>96</v>
       </c>
       <c r="J13" s="4" t="n">
         <v>6</v>
@@ -1468,19 +1502,19 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>95</v>
+        <v>98</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="J14" s="4" t="n">
         <v>7</v>
@@ -1488,19 +1522,19 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>98</v>
+        <v>101</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="J15" s="4" t="n">
         <v>7</v>
@@ -1508,19 +1542,19 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>101</v>
+        <v>104</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="J16" s="4" t="n">
         <v>8</v>
@@ -1528,19 +1562,19 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>108</v>
       </c>
       <c r="J17" s="4" t="n">
         <v>8</v>
@@ -1548,19 +1582,19 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>107</v>
+        <v>110</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="J18" s="4" t="n">
         <v>9</v>
@@ -1584,8 +1618,8 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1593,9 +1627,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="224.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="8.54"/>
@@ -1604,61 +1639,61 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="D1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>35</v>
+      <c r="H1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>110</v>
+        <v>113</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1704,15 +1739,15 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>12</v>
@@ -1720,51 +1755,51 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -1772,46 +1807,46 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>127</v>
+        <v>130</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Updates PfR shiny xlxs
</commit_message>
<xml_diff>
--- a/PfR_Shiny.xlsx
+++ b/PfR_Shiny.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="138">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -842,15 +842,15 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="68.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="68.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.54"/>
@@ -991,8 +991,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1174,9 +1174,7 @@
       <c r="C7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
         <v>59</v>
       </c>

</xml_diff>